<commit_message>
feat: subtract EV/PHV electricity consumption from housing
</commit_message>
<xml_diff>
--- a/src/tests/other-estimation.test-cases.xlsx
+++ b/src/tests/other-estimation.test-cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF67B10-E9AA-134A-B3C6-84DDFEEAA4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D5C8C9-13FC-414E-B7C2-493359AF5F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="7700" windowWidth="38400" windowHeight="21100" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="10" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
     <sheet name="answers" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8792" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8792" uniqueCount="261">
   <si>
     <t>case</t>
     <phoneticPr fontId="2"/>
@@ -1425,6 +1425,10 @@
     <t>otherE7</t>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>10k-30k</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
@@ -2496,8 +2500,8 @@
   </sheetPr>
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -3435,7 +3439,7 @@
         <v>15</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>203</v>
@@ -6434,8 +6438,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -7326,7 +7330,7 @@
         <v>80</v>
       </c>
       <c r="D23" s="12">
-        <v>21.032396769743837</v>
+        <v>16.825917415795068</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>21</v>
@@ -7365,7 +7369,7 @@
         <v>80</v>
       </c>
       <c r="D24" s="12">
-        <v>3.9676032302561621</v>
+        <v>3.1740825842049296</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>21</v>

</xml_diff>